<commit_message>
Add miss rate estimation, add dummy cache
</commit_message>
<xml_diff>
--- a/Final/results.xlsx
+++ b/Final/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorhuang/Desktop/DSD/Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4C655466-9F28-4548-B89E-6EAC15E4F68D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B1177528-BDDE-A84B-9DB1-78B481A304EC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="1320" windowWidth="18040" windowHeight="13800" xr2:uid="{299BFB76-7EC4-FE4D-A66F-EE798D0970FC}"/>
+    <workbookView xWindow="5880" yWindow="1780" windowWidth="23000" windowHeight="9680" xr2:uid="{299BFB76-7EC4-FE4D-A66F-EE798D0970FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,22 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
-  <si>
-    <t>L2Cache</t>
-  </si>
-  <si>
-    <t>baseline</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>T (ns)</t>
-  </si>
-  <si>
-    <t>A (cell area)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>HW4</t>
   </si>
@@ -85,6 +70,51 @@
   </si>
   <si>
     <t>area</t>
+  </si>
+  <si>
+    <t>Cache</t>
+  </si>
+  <si>
+    <t>nb</t>
+  </si>
+  <si>
+    <t>no cache</t>
+  </si>
+  <si>
+    <t>+I+D</t>
+  </si>
+  <si>
+    <t>+I+L2D</t>
+  </si>
+  <si>
+    <t>+I</t>
+  </si>
+  <si>
+    <t>+D</t>
+  </si>
+  <si>
+    <t>+L2I+L2D</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>L2I</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>L2D</t>
+  </si>
+  <si>
+    <t>write miss rate</t>
+  </si>
+  <si>
+    <t>L1 vs. L2</t>
+  </si>
+  <si>
+    <t>L2 size</t>
   </si>
 </sst>
 </file>
@@ -129,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -148,6 +178,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,272 +499,575 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4F9896-A7F8-294F-A3AD-69DB43562484}">
-  <dimension ref="B3:K23"/>
+  <dimension ref="A2:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="116" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.83203125" style="1"/>
+    <col min="12" max="17" width="16" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>4</v>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="7"/>
+      <c r="P2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
+        <v>16</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
         <v>5</v>
       </c>
-      <c r="E4" s="2">
-        <f>8843/5</f>
-        <v>1768.6</v>
+      <c r="C4" s="1">
+        <v>13187</v>
+      </c>
+      <c r="D4" s="2">
+        <v>9148</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5231</v>
       </c>
       <c r="F4" s="2">
-        <f>8003/5</f>
-        <v>1600.6</v>
-      </c>
-      <c r="G4" s="3">
-        <f>(F4-E4)/E4</f>
-        <v>-9.4990387877417176E-2</v>
-      </c>
-      <c r="J4" s="1">
-        <v>287356</v>
+        <v>1830</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1830</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1601</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="K4" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D5" s="1">
+      <c r="L4" s="3">
+        <f>59/1407</f>
+        <v>4.1933191186922528E-2</v>
+      </c>
+      <c r="M4" s="3">
+        <f>19/1419</f>
+        <v>1.3389711064129669E-2</v>
+      </c>
+      <c r="N4" s="3">
+        <f>5/196</f>
+        <v>2.5510204081632654E-2</v>
+      </c>
+      <c r="O4" s="3">
+        <f>0/194</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <f>5/196</f>
+        <v>2.5510204081632654E-2</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>0/194</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
         <v>10</v>
       </c>
-      <c r="E5" s="2">
-        <f>39913/5</f>
-        <v>7982.6</v>
+      <c r="C5" s="1">
+        <v>70483</v>
+      </c>
+      <c r="D5" s="2">
+        <v>46059</v>
+      </c>
+      <c r="E5" s="1">
+        <v>28942</v>
       </c>
       <c r="F5" s="2">
-        <f>37158/5</f>
-        <v>7431.6</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" ref="G5:G9" si="0">(F5-E5)/E5</f>
-        <v>-6.9025129657003984E-2</v>
+        <v>8130</v>
+      </c>
+      <c r="G5" s="2">
+        <v>7991</v>
+      </c>
+      <c r="H5" s="1">
+        <v>6832</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="K5" s="1">
+        <v>10</v>
+      </c>
+      <c r="L5" s="3">
+        <f>119/7287</f>
+        <v>1.633045148895293E-2</v>
+      </c>
+      <c r="M5" s="3">
+        <f>19/7190</f>
+        <v>2.6425591098748263E-3</v>
+      </c>
+      <c r="N5" s="3">
+        <f>33/1156</f>
+        <v>2.8546712802768166E-2</v>
+      </c>
+      <c r="O5" s="3">
+        <f>21/1184</f>
+        <v>1.7736486486486486E-2</v>
+      </c>
+      <c r="P5" s="3">
+        <f>10/1156</f>
+        <v>8.6505190311418692E-3</v>
+      </c>
+      <c r="Q5" s="3">
+        <f>0/1184</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
+        <v>111895</v>
+      </c>
+      <c r="E6" s="8">
+        <v>71577</v>
+      </c>
+      <c r="F6" s="8">
+        <v>19725</v>
+      </c>
+      <c r="G6" s="8">
+        <v>18686</v>
+      </c>
+      <c r="H6" s="1">
+        <v>17797</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="K6" s="1">
+        <v>15</v>
+      </c>
+      <c r="L6" s="3">
+        <f>179/18462</f>
+        <v>9.6955909435597447E-3</v>
+      </c>
+      <c r="M6" s="3">
+        <f>19/17495</f>
+        <v>1.086024578450986E-3</v>
+      </c>
+      <c r="N6" s="3">
+        <f>188/2916</f>
+        <v>6.4471879286694095E-2</v>
+      </c>
+      <c r="O6" s="3">
+        <f>176/2984</f>
+        <v>5.8981233243967826E-2</v>
+      </c>
+      <c r="P6" s="3">
+        <f>15/2916</f>
+        <v>5.1440329218106996E-3</v>
+      </c>
+      <c r="Q6" s="3">
+        <f>0/2984</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8">
+        <v>133012</v>
+      </c>
+      <c r="F7" s="8">
+        <v>37068</v>
+      </c>
+      <c r="G7" s="8">
+        <v>33972</v>
+      </c>
+      <c r="H7" s="1">
+        <v>32753</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="K7" s="1">
+        <v>20</v>
+      </c>
+      <c r="L7" s="3">
+        <f>239/35385</f>
+        <v>6.7542744100607599E-3</v>
+      </c>
+      <c r="M7" s="3">
+        <f>19/32391</f>
+        <v>5.8658269272328736E-4</v>
+      </c>
+      <c r="N7" s="3">
+        <f>535/5476</f>
+        <v>9.7699050401753099E-2</v>
+      </c>
+      <c r="O7" s="3">
+        <f>516/5584</f>
+        <v>9.2406876790830941E-2</v>
+      </c>
+      <c r="P7" s="3">
+        <f>20/5476</f>
+        <v>3.6523009495982471E-3</v>
+      </c>
+      <c r="Q7" s="3">
+        <f>0/5584</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>25</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8">
+        <v>59495</v>
+      </c>
+      <c r="G8" s="8">
+        <v>53757</v>
+      </c>
+      <c r="H8" s="1">
+        <v>52208</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="1">
+        <v>25</v>
+      </c>
+      <c r="L8" s="3">
+        <f>299/57392</f>
+        <v>5.2097853359353219E-3</v>
+      </c>
+      <c r="M8" s="3">
+        <f>19/51786</f>
+        <v>3.6689452747846909E-4</v>
+      </c>
+      <c r="N8" s="3">
+        <f>981/8836</f>
+        <v>0.11102308736985061</v>
+      </c>
+      <c r="O8" s="3">
+        <f>956/8984</f>
+        <v>0.10641139804096171</v>
+      </c>
+      <c r="P8" s="3">
+        <f>25/8836</f>
+        <v>2.8293345405160705E-3</v>
+      </c>
+      <c r="Q8" s="3">
+        <f>0/8984</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>30</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8">
+        <v>87050</v>
+      </c>
+      <c r="G9" s="8">
+        <v>78045</v>
+      </c>
+      <c r="H9" s="1">
+        <v>76166</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="K9" s="1">
+        <v>30</v>
+      </c>
+      <c r="L9" s="3">
+        <f>359/84527</f>
+        <v>4.2471636281898092E-3</v>
+      </c>
+      <c r="M9" s="3">
+        <f>19/75684</f>
+        <v>2.5104381375191584E-4</v>
+      </c>
+      <c r="N9" s="3">
+        <f>1529/12996</f>
+        <v>0.11765158510310865</v>
+      </c>
+      <c r="O9" s="3">
+        <f>1497/13184</f>
+        <v>0.11354672330097088</v>
+      </c>
+      <c r="P9" s="3">
+        <f>30/12996</f>
+        <v>2.3084025854108957E-3</v>
+      </c>
+      <c r="Q9" s="3">
+        <f>0/13184</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3">
+        <f>N9</f>
+        <v>0.11765158510310865</v>
+      </c>
+      <c r="M13" s="3">
+        <f>O9</f>
+        <v>0.11354672330097088</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6161</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4182</v>
+      </c>
+      <c r="F14" s="3">
+        <f>(E14-D14)/D14</f>
+        <v>-0.32121408862197698</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="K14" s="1">
+        <v>16</v>
+      </c>
+      <c r="L14" s="3">
+        <f>1231/12996</f>
+        <v>9.472145275469375E-2</v>
+      </c>
+      <c r="M14" s="3">
+        <f>730/13184</f>
+        <v>5.5370145631067964E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="K15" s="1">
+        <v>32</v>
+      </c>
+      <c r="L15" s="3">
+        <f>30/12996</f>
+        <v>2.3084025854108957E-3</v>
+      </c>
+      <c r="M15" s="3">
+        <f>0/13184</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D6" s="1">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2">
-        <f>96838/5</f>
-        <v>19367.599999999999</v>
-      </c>
-      <c r="F6" s="2">
-        <f>88983/5</f>
-        <v>17796.599999999999</v>
-      </c>
-      <c r="G6" s="3">
-        <f t="shared" si="0"/>
-        <v>-8.1114851607839905E-2</v>
-      </c>
-      <c r="K6" s="1">
+      <c r="E16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="1">
+        <v>64</v>
+      </c>
+      <c r="L16" s="3">
+        <f>30/12996</f>
+        <v>2.3084025854108957E-3</v>
+      </c>
+      <c r="M16" s="3">
+        <f>0/13184</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D7" s="1">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2">
-        <f>181523/5</f>
-        <v>36304.6</v>
-      </c>
-      <c r="F7" s="2">
-        <f>163763/5</f>
-        <v>32752.6</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" si="0"/>
-        <v>-9.7838841358946257E-2</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="C17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2065</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2074</v>
+      </c>
+      <c r="K17" s="1">
+        <v>128</v>
+      </c>
+      <c r="L17" s="3">
+        <f>30/12996</f>
+        <v>2.3084025854108957E-3</v>
+      </c>
+      <c r="M17" s="3">
+        <f>0/13184</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D8" s="1">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2">
-        <f>291153/5</f>
-        <v>58230.6</v>
-      </c>
-      <c r="F8" s="2">
-        <f>261038/5</f>
-        <v>52207.6</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.10343358989946867</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D9" s="1">
-        <v>30</v>
-      </c>
-      <c r="E9" s="2">
-        <f>425893/5</f>
-        <v>85178.6</v>
-      </c>
-      <c r="F9" s="2">
-        <f>380828/5</f>
-        <v>76165.600000000006</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.10581296241074635</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1">
-        <v>6161</v>
-      </c>
-      <c r="E13" s="1">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
         <v>4182</v>
       </c>
-      <c r="F13" s="3">
-        <f>(E13-D13)/D13</f>
-        <v>-0.32121408862197698</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C14" s="4" t="s">
+      <c r="E20" s="1">
+        <v>8811</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="E22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="1">
-        <v>2065</v>
-      </c>
-      <c r="E16" s="1">
-        <v>2074</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D18" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="1">
-        <v>4182</v>
-      </c>
-      <c r="E19" s="1">
-        <v>8811</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="D23" s="1">
         <v>738854</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E23" s="1">
         <v>406828</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="1">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1">
         <v>188</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E24" s="1">
         <v>512</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="O4:P4" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>